<commit_message>
new test for tmp reader and update old
</commit_message>
<xml_diff>
--- a/tox5_preprocessing/test/test_data/HARMLESS_for_tests.xlsx
+++ b/tox5_preprocessing/test/test_data/HARMLESS_for_tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="18090" windowHeight="4575" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="18090" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="ctg_normalization" sheetId="11" r:id="rId1"/>
@@ -1731,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GF147"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BK25" sqref="BK25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,7 +1808,7 @@
       </c>
       <c r="AO1" s="13">
         <f>AO3+2*AO2</f>
-        <v>12.382357400485215</v>
+        <v>13.864309976288093</v>
       </c>
       <c r="AP1" s="13">
         <f>AP3+2*AP2</f>
@@ -1820,19 +1820,19 @@
       </c>
       <c r="AR1" s="13">
         <f t="shared" si="0"/>
-        <v>15.371283799459114</v>
+        <v>16.086964090972184</v>
       </c>
       <c r="AS1" s="13">
         <f t="shared" si="0"/>
-        <v>19.152425247981597</v>
+        <v>17.380400096054011</v>
       </c>
       <c r="AT1" s="13">
         <f t="shared" si="0"/>
-        <v>17.78832539481424</v>
+        <v>16.4813699472612</v>
       </c>
       <c r="AU1" s="13">
         <f t="shared" si="0"/>
-        <v>17.670039165783511</v>
+        <v>16.592951769361118</v>
       </c>
       <c r="AX1" s="24" t="s">
         <v>27</v>
@@ -1844,15 +1844,15 @@
       </c>
       <c r="BA1" s="26">
         <f t="shared" ref="BA1" si="1">BA4+3*BA3</f>
-        <v>20.087054355460761</v>
+        <v>21.792445276702246</v>
       </c>
       <c r="BB1" s="26">
         <f>BB4+3*BB3</f>
-        <v>24.91197560066038</v>
+        <v>25.248272702711606</v>
       </c>
       <c r="BC1" s="26">
         <f t="shared" ref="BC1" si="2">BC4+3*BC3</f>
-        <v>25.581855156010441</v>
+        <v>24.679338117544827</v>
       </c>
       <c r="BD1" s="84"/>
       <c r="BF1" s="23" t="s">
@@ -1990,7 +1990,7 @@
       </c>
       <c r="AO2" s="29">
         <f t="shared" ref="AO2:AU2" si="3">STDEV(AO17:AO24)</f>
-        <v>6.3678221903046293</v>
+        <v>6.5674534673923537</v>
       </c>
       <c r="AP2" s="29">
         <f t="shared" si="3"/>
@@ -2002,19 +2002,19 @@
       </c>
       <c r="AR2" s="29">
         <f t="shared" si="3"/>
-        <v>7.903826048016521</v>
+        <v>7.208569834879234</v>
       </c>
       <c r="AS2" s="29">
         <f t="shared" si="3"/>
-        <v>10.351492734767985</v>
+        <v>9.4631832620896628</v>
       </c>
       <c r="AT2" s="29">
         <f t="shared" si="3"/>
-        <v>9.496744851171206</v>
+        <v>8.8432671273946859</v>
       </c>
       <c r="AU2" s="29">
         <f t="shared" si="3"/>
-        <v>8.0138025035328333</v>
+        <v>6.1775457951009969</v>
       </c>
       <c r="AX2" s="24" t="s">
         <v>29</v>
@@ -2026,15 +2026,15 @@
       </c>
       <c r="BA2" s="28">
         <f t="shared" ref="BA2" si="4">BA4+2*BA3</f>
-        <v>13.273607243599161</v>
+        <v>14.771431198302626</v>
       </c>
       <c r="BB2" s="28">
         <f>BB4+2*BB3</f>
-        <v>16.46252763491561</v>
+        <v>17.388789942212309</v>
       </c>
       <c r="BC2" s="28">
         <f t="shared" ref="BC2" si="5">BC4+2*BC3</f>
-        <v>16.638077055698833</v>
+        <v>17.000370131269165</v>
       </c>
       <c r="BD2" s="85"/>
       <c r="BF2" s="31" t="s">
@@ -2079,7 +2079,7 @@
       </c>
       <c r="AO3" s="29">
         <f t="shared" ref="AO3:AU3" si="6">MEDIAN(AO17:AO24)</f>
-        <v>-0.35328698012404292</v>
+        <v>0.72940304150338475</v>
       </c>
       <c r="AP3" s="29">
         <f t="shared" si="6"/>
@@ -2091,11 +2091,11 @@
       </c>
       <c r="AR3" s="29">
         <f t="shared" si="6"/>
-        <v>-0.43636829657392706</v>
+        <v>1.669824421213717</v>
       </c>
       <c r="AS3" s="29">
         <f t="shared" si="6"/>
-        <v>-1.5505602215543726</v>
+        <v>-1.5459664281253165</v>
       </c>
       <c r="AT3" s="29">
         <f t="shared" si="6"/>
@@ -2103,7 +2103,7 @@
       </c>
       <c r="AU3" s="29">
         <f t="shared" si="6"/>
-        <v>1.6424341587178426</v>
+        <v>4.2378601791591253</v>
       </c>
       <c r="AX3" s="24" t="s">
         <v>35</v>
@@ -2115,15 +2115,15 @@
       </c>
       <c r="BA3" s="29">
         <f>STDEV(AO17:AO24,AQ17:AQ24)</f>
-        <v>6.8134471118616018</v>
+        <v>7.0210140783996202</v>
       </c>
       <c r="BB3" s="29">
         <f>STDEV(AR17:AR24,AT17:AT24)</f>
-        <v>8.4494479657447688</v>
+        <v>7.8594827604992963</v>
       </c>
       <c r="BC3" s="29">
         <f>STDEV(AS17:AS24,AU17:AU24)</f>
-        <v>8.9437781003116061</v>
+        <v>7.6789679862756612</v>
       </c>
       <c r="BD3" s="29"/>
       <c r="BF3" s="32" t="s">
@@ -2217,15 +2217,15 @@
       </c>
       <c r="BA4" s="29">
         <f>MEDIAN(AO17:AO24,AQ17:AQ24)</f>
-        <v>-0.35328698012404292</v>
+        <v>0.72940304150338475</v>
       </c>
       <c r="BB4" s="29">
         <f>MEDIAN(AR17:AR24,AT17:AT24)</f>
-        <v>-0.43636829657392706</v>
+        <v>1.669824421213717</v>
       </c>
       <c r="BC4" s="29">
         <f>MEDIAN(AS17:AS24,AU17:AU24)</f>
-        <v>-1.2494791449243781</v>
+        <v>1.6424341587178426</v>
       </c>
       <c r="BD4" s="29"/>
       <c r="BG4" s="13"/>
@@ -5189,9 +5189,9 @@
         <f t="shared" si="49"/>
         <v/>
       </c>
-      <c r="BZ11" s="68">
+      <c r="BZ11" s="68" t="str">
         <f t="shared" si="50"/>
-        <v>1.2810131992300086E-2</v>
+        <v/>
       </c>
       <c r="CA11" s="68" t="str">
         <f t="shared" si="51"/>
@@ -5213,7 +5213,7 @@
       </c>
       <c r="CG11" s="69">
         <f t="shared" si="54"/>
-        <v>1.2810131992300086E-2</v>
+        <v>0</v>
       </c>
       <c r="CH11" s="69">
         <f t="shared" si="55"/>
@@ -5370,13 +5370,13 @@
         <f>IF($AZ11&lt;$AZ$2,"",AP11)</f>
         <v/>
       </c>
-      <c r="FA11" s="66">
+      <c r="FA11" s="66" t="str">
         <f>IF($BA11&lt;$BA$2,"",AO11)</f>
-        <v>12.873464969119507</v>
-      </c>
-      <c r="FB11" s="66">
+        <v/>
+      </c>
+      <c r="FB11" s="66" t="str">
         <f t="shared" si="64"/>
-        <v>14.019854495986305</v>
+        <v/>
       </c>
       <c r="FC11" s="66" t="str">
         <f t="shared" si="65"/>
@@ -8227,7 +8227,7 @@
         <v>4.1101527517794727</v>
       </c>
       <c r="AR17" s="131">
-        <f t="shared" si="24"/>
+        <f>AA17-$AJ17</f>
         <v>-2.5425610143615711</v>
       </c>
       <c r="AS17" s="131">
@@ -8235,7 +8235,7 @@
         <v>-1.5459664281253165</v>
       </c>
       <c r="AT17" s="131">
-        <f t="shared" si="26"/>
+        <f>AD17-$AJ17</f>
         <v>-11.027464311455951</v>
       </c>
       <c r="AU17" s="131">
@@ -8723,10 +8723,7 @@
         <f t="shared" si="25"/>
         <v>11.329433041431558</v>
       </c>
-      <c r="AT18" s="66">
-        <f t="shared" si="26"/>
-        <v>8.409163559706446</v>
-      </c>
+      <c r="AT18" s="66"/>
       <c r="AU18" s="66">
         <f t="shared" si="27"/>
         <v>8.409163559706446</v>
@@ -8750,7 +8747,7 @@
       </c>
       <c r="BB18" s="67">
         <f t="shared" si="43"/>
-        <v>8.0384852530480906</v>
+        <v>7.6678069463897334</v>
       </c>
       <c r="BC18" s="67">
         <f t="shared" si="44"/>
@@ -9169,10 +9166,7 @@
         <f t="shared" si="23"/>
         <v>-9.2617255958193709</v>
       </c>
-      <c r="AR19" s="66">
-        <f>AA19-$AJ19</f>
-        <v>4.7177227554796808</v>
-      </c>
+      <c r="AR19" s="66"/>
       <c r="AS19" s="66">
         <f t="shared" si="25"/>
         <v>-1.5551540149834286</v>
@@ -9204,7 +9198,7 @@
       </c>
       <c r="BB19" s="67">
         <f t="shared" si="43"/>
-        <v>3.4305651879646182</v>
+        <v>2.1434076204495556</v>
       </c>
       <c r="BC19" s="67">
         <f t="shared" si="44"/>
@@ -9611,10 +9605,7 @@
         <f t="shared" si="20"/>
         <v>-4.4877419098711515</v>
       </c>
-      <c r="AO20" s="66">
-        <f t="shared" si="21"/>
-        <v>-0.18794274974699987</v>
-      </c>
+      <c r="AO20" s="66"/>
       <c r="AP20" s="66">
         <f t="shared" si="22"/>
         <v>5.2834450088886147</v>
@@ -9623,10 +9614,7 @@
         <f t="shared" si="23"/>
         <v>-1.5419507796514631</v>
       </c>
-      <c r="AR20" s="66">
-        <f t="shared" si="24"/>
-        <v>-4.504348360407084</v>
-      </c>
+      <c r="AR20" s="66"/>
       <c r="AS20" s="66">
         <f t="shared" si="25"/>
         <v>-7.644765314414836</v>
@@ -9654,11 +9642,11 @@
       </c>
       <c r="BA20" s="67">
         <f t="shared" si="42"/>
-        <v>-0.86494676469923149</v>
+        <v>-1.5419507796514631</v>
       </c>
       <c r="BB20" s="67">
         <f t="shared" si="43"/>
-        <v>-4.5270152861243353</v>
+        <v>-4.5496822118415876</v>
       </c>
       <c r="BC20" s="67">
         <f t="shared" si="44"/>
@@ -11433,10 +11421,7 @@
         <f t="shared" si="20"/>
         <v>11.012013674322439</v>
       </c>
-      <c r="AO24" s="66">
-        <f t="shared" si="21"/>
-        <v>-7.6295784381478882</v>
-      </c>
+      <c r="AO24" s="66"/>
       <c r="AP24" s="66">
         <f t="shared" si="22"/>
         <v>11.805968267765021</v>
@@ -11445,22 +11430,10 @@
         <f t="shared" si="23"/>
         <v>9.0310888746030429</v>
       </c>
-      <c r="AR24" s="66">
-        <f t="shared" si="24"/>
-        <v>-13.381954679152912</v>
-      </c>
-      <c r="AS24" s="66">
-        <f t="shared" si="25"/>
-        <v>-13.381954679152912</v>
-      </c>
-      <c r="AT24" s="66">
-        <f t="shared" si="26"/>
-        <v>-13.381954679152912</v>
-      </c>
-      <c r="AU24" s="66">
-        <f t="shared" si="27"/>
-        <v>-13.381954679152912</v>
-      </c>
+      <c r="AR24" s="66"/>
+      <c r="AS24" s="66"/>
+      <c r="AT24" s="66"/>
+      <c r="AU24" s="66"/>
       <c r="AW24" s="4" t="s">
         <v>68</v>
       </c>
@@ -11476,15 +11449,15 @@
       </c>
       <c r="BA24" s="67">
         <f t="shared" si="42"/>
-        <v>0.70075521822757736</v>
-      </c>
-      <c r="BB24" s="67">
+        <v>9.0310888746030429</v>
+      </c>
+      <c r="BB24" s="67" t="e">
         <f t="shared" si="43"/>
-        <v>-13.381954679152912</v>
-      </c>
-      <c r="BC24" s="67">
+        <v>#NUM!</v>
+      </c>
+      <c r="BC24" s="67" t="e">
         <f t="shared" si="44"/>
-        <v>-13.381954679152912</v>
+        <v>#NUM!</v>
       </c>
       <c r="BD24" s="67"/>
       <c r="BE24" s="4" t="s">
@@ -11553,13 +11526,13 @@
         <f t="shared" si="50"/>
         <v/>
       </c>
-      <c r="CA24" s="68" t="str">
+      <c r="CA24" s="68" t="e">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="CB24" s="68" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="CB24" s="68" t="e">
         <f t="shared" si="52"/>
-        <v/>
+        <v>#NUM!</v>
       </c>
       <c r="CD24" s="4" t="s">
         <v>68</v>
@@ -11575,13 +11548,13 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="CH24" s="69">
+      <c r="CH24" s="69" t="e">
         <f t="shared" si="55"/>
-        <v>0</v>
-      </c>
-      <c r="CI24" s="69">
+        <v>#NUM!</v>
+      </c>
+      <c r="CI24" s="69" t="e">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="CK24" s="4" t="s">
         <v>68</v>
@@ -11625,13 +11598,13 @@
         <f t="shared" si="73"/>
         <v/>
       </c>
-      <c r="DC24" s="68" t="str">
+      <c r="DC24" s="68" t="e">
         <f t="shared" si="73"/>
-        <v/>
-      </c>
-      <c r="DD24" s="68" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="DD24" s="68" t="e">
         <f t="shared" si="73"/>
-        <v/>
+        <v>#NUM!</v>
       </c>
       <c r="DF24" s="4" t="s">
         <v>68</v>
@@ -11647,13 +11620,13 @@
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="DJ24" s="69">
+      <c r="DJ24" s="69" t="e">
         <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="DK24" s="69">
+        <v>#NUM!</v>
+      </c>
+      <c r="DK24" s="69" t="e">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="DM24" s="63" t="s">
         <v>68</v>
@@ -11712,21 +11685,21 @@
         <f>IF($BA24&lt;$BA$2,"",#REF!)</f>
         <v/>
       </c>
-      <c r="FC24" s="66" t="str">
+      <c r="FC24" s="66" t="e">
         <f>IF($BB24&lt;$BB$2,"",#REF!)</f>
-        <v/>
-      </c>
-      <c r="FD24" s="66" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="FD24" s="66" t="e">
         <f>IF($BB24&lt;$BB$2,"",#REF!)</f>
-        <v/>
-      </c>
-      <c r="FE24" s="66" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="FE24" s="66" t="e">
         <f>IF($BC24&lt;$BC$2,"",#REF!)</f>
-        <v/>
-      </c>
-      <c r="FF24" s="66" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="FF24" s="66" t="e">
         <f>IF($BC24&lt;$BC$2,"",#REF!)</f>
-        <v/>
+        <v>#NUM!</v>
       </c>
       <c r="FH24" s="63" t="s">
         <v>68</v>
@@ -19378,8 +19351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>